<commit_message>
adjusting data label positions
</commit_message>
<xml_diff>
--- a/docs/figdata.xlsx
+++ b/docs/figdata.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t xml:space="preserve">year</t>
   </si>
@@ -23,7 +23,7 @@
     <t xml:space="preserve">sex</t>
   </si>
   <si>
-    <t xml:space="preserve">goodsp_lbl</t>
+    <t xml:space="preserve">goodsp</t>
   </si>
   <si>
     <t xml:space="preserve">vals</t>
@@ -38,25 +38,25 @@
     <t xml:space="preserve">Men</t>
   </si>
   <si>
-    <t xml:space="preserve">Very
-good</t>
+    <t xml:space="preserve">Very good</t>
   </si>
   <si>
     <t xml:space="preserve">Good</t>
   </si>
   <si>
-    <t xml:space="preserve">Fairly
-good</t>
+    <t xml:space="preserve">Fairly good</t>
   </si>
   <si>
-    <t xml:space="preserve">Not so
-good</t>
+    <t xml:space="preserve">Not so good</t>
   </si>
   <si>
     <t xml:space="preserve">Poor</t>
   </si>
   <si>
     <t xml:space="preserve">Women</t>
+  </si>
+  <si>
+    <t xml:space="preserve">goodsp_lbl</t>
   </si>
   <si>
     <t xml:space="preserve">vals_2012</t>
@@ -83,10 +83,22 @@
     <t xml:space="preserve">label</t>
   </si>
   <si>
+    <t xml:space="preserve">Very
+good</t>
+  </si>
+  <si>
     <t xml:space="preserve">-8%</t>
   </si>
   <si>
     <t xml:space="preserve">1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fairly
+good</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not so
+good</t>
   </si>
   <si>
     <t xml:space="preserve">2%</t>
@@ -9902,31 +9914,31 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2">
@@ -9934,7 +9946,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C2" t="n">
         <v>0.595693316027162</v>
@@ -9958,7 +9970,7 @@
         <v>-0.0782702540189268</v>
       </c>
       <c r="J2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3">
@@ -9990,7 +10002,7 @@
         <v>0.0131073404247971</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4">
@@ -9998,7 +10010,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C4" t="n">
         <v>0.0658866514706961</v>
@@ -10022,7 +10034,7 @@
         <v>0.0135955425068847</v>
       </c>
       <c r="J4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
@@ -10030,7 +10042,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C5" t="n">
         <v>0.0113092777324113</v>
@@ -10054,7 +10066,7 @@
         <v>0.0203483969796505</v>
       </c>
       <c r="J5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6">
@@ -10086,7 +10098,7 @@
         <v>0.0312189741075945</v>
       </c>
       <c r="J6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
@@ -10094,7 +10106,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C7" t="n">
         <v>0.638594482334447</v>
@@ -10118,7 +10130,7 @@
         <v>-0.108234950987242</v>
       </c>
       <c r="J7" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8">
@@ -10150,7 +10162,7 @@
         <v>-0.0084015219880455</v>
       </c>
       <c r="J8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9">
@@ -10158,7 +10170,7 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C9" t="n">
         <v>0.0672562937219824</v>
@@ -10182,7 +10194,7 @@
         <v>0.0954716360139245</v>
       </c>
       <c r="J9" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10">
@@ -10190,7 +10202,7 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C10" t="n">
         <v>0.016615937030459</v>
@@ -10214,7 +10226,7 @@
         <v>0.00132774227729436</v>
       </c>
       <c r="J10" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11">
@@ -10246,7 +10258,7 @@
         <v>0.0198370946840692</v>
       </c>
       <c r="J11" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -10271,7 +10283,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -10291,7 +10303,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D2" t="n">
         <v>0.726769075663697</v>
@@ -10311,7 +10323,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D3" t="n">
         <v>0.217325610962265</v>
@@ -10331,7 +10343,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D4" t="n">
         <v>0.0559053133740384</v>
@@ -10351,7 +10363,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D5" t="n">
         <v>0.836504580865343</v>
@@ -10371,7 +10383,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D6" t="n">
         <v>0.116513976911448</v>
@@ -10391,7 +10403,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D7" t="n">
         <v>0.0469814422232094</v>
@@ -10411,7 +10423,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D8" t="n">
         <v>0.750119104138274</v>
@@ -10431,7 +10443,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D9" t="n">
         <v>0.200095283689241</v>
@@ -10451,7 +10463,7 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D10" t="n">
         <v>0.0497856121724848</v>
@@ -10471,7 +10483,7 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D11" t="n">
         <v>0.818546683642975</v>
@@ -10491,7 +10503,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D12" t="n">
         <v>0.135192226431908</v>
@@ -10511,7 +10523,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D13" t="n">
         <v>0.0462610899251166</v>
@@ -10531,7 +10543,7 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D14" t="n">
         <v>0.752206809588835</v>
@@ -10551,7 +10563,7 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D15" t="n">
         <v>0.196931484017206</v>
@@ -10571,7 +10583,7 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D16" t="n">
         <v>0.050861706393959</v>
@@ -10591,7 +10603,7 @@
         <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D17" t="n">
         <v>0.825733474800192</v>
@@ -10611,7 +10623,7 @@
         <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D18" t="n">
         <v>0.121597737689063</v>
@@ -10631,7 +10643,7 @@
         <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D19" t="n">
         <v>0.0526687875107446</v>
@@ -10651,7 +10663,7 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D20" t="n">
         <v>0.752920432263023</v>
@@ -10671,7 +10683,7 @@
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D21" t="n">
         <v>0.190654617371408</v>
@@ -10691,7 +10703,7 @@
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D22" t="n">
         <v>0.0564249503655692</v>
@@ -10711,7 +10723,7 @@
         <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D23" t="n">
         <v>0.850461409474052</v>
@@ -10731,7 +10743,7 @@
         <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D24" t="n">
         <v>0.10927013433273</v>
@@ -10751,7 +10763,7 @@
         <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D25" t="n">
         <v>0.0402684561932184</v>
@@ -10771,7 +10783,7 @@
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D26" t="n">
         <v>0.763915962959485</v>
@@ -10791,7 +10803,7 @@
         <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D27" t="n">
         <v>0.184968593804611</v>
@@ -10811,7 +10823,7 @@
         <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D28" t="n">
         <v>0.0511154432359035</v>
@@ -10831,7 +10843,7 @@
         <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D29" t="n">
         <v>0.853618756292581</v>
@@ -10851,7 +10863,7 @@
         <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D30" t="n">
         <v>0.108664627808067</v>
@@ -10871,7 +10883,7 @@
         <v>12</v>
       </c>
       <c r="C31" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D31" t="n">
         <v>0.0377166158993521</v>
@@ -10891,7 +10903,7 @@
         <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D32" t="n">
         <v>0.776300351803189</v>
@@ -10911,7 +10923,7 @@
         <v>6</v>
       </c>
       <c r="C33" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D33" t="n">
         <v>0.182831443298295</v>
@@ -10931,7 +10943,7 @@
         <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D34" t="n">
         <v>0.0408682048985154</v>
@@ -10951,7 +10963,7 @@
         <v>12</v>
       </c>
       <c r="C35" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D35" t="n">
         <v>0.836173000990399</v>
@@ -10971,7 +10983,7 @@
         <v>12</v>
       </c>
       <c r="C36" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D36" t="n">
         <v>0.123385134359978</v>
@@ -10991,7 +11003,7 @@
         <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D37" t="n">
         <v>0.0404418646496229</v>
@@ -11011,7 +11023,7 @@
         <v>6</v>
       </c>
       <c r="C38" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D38" t="n">
         <v>0.75257731956182</v>
@@ -11031,7 +11043,7 @@
         <v>6</v>
       </c>
       <c r="C39" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D39" t="n">
         <v>0.192248950146891</v>
@@ -11051,7 +11063,7 @@
         <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D40" t="n">
         <v>0.0551737302912889</v>
@@ -11071,7 +11083,7 @@
         <v>12</v>
       </c>
       <c r="C41" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D41" t="n">
         <v>0.839159538954733</v>
@@ -11091,7 +11103,7 @@
         <v>12</v>
       </c>
       <c r="C42" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D42" t="n">
         <v>0.116957976989298</v>
@@ -11111,7 +11123,7 @@
         <v>12</v>
       </c>
       <c r="C43" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D43" t="n">
         <v>0.0438824840559692</v>
@@ -11131,7 +11143,7 @@
         <v>6</v>
       </c>
       <c r="C44" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D44" t="n">
         <v>0.757607337477793</v>
@@ -11151,7 +11163,7 @@
         <v>6</v>
       </c>
       <c r="C45" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D45" t="n">
         <v>0.181325551545777</v>
@@ -11171,7 +11183,7 @@
         <v>6</v>
       </c>
       <c r="C46" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D46" t="n">
         <v>0.0610671109764305</v>
@@ -11191,7 +11203,7 @@
         <v>12</v>
       </c>
       <c r="C47" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D47" t="n">
         <v>0.850249252722757</v>
@@ -11211,7 +11223,7 @@
         <v>12</v>
       </c>
       <c r="C48" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D48" t="n">
         <v>0.11046859381806</v>
@@ -11231,7 +11243,7 @@
         <v>12</v>
       </c>
       <c r="C49" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D49" t="n">
         <v>0.0392821534591829</v>
@@ -11251,7 +11263,7 @@
         <v>6</v>
       </c>
       <c r="C50" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D50" t="n">
         <v>0.735646687426739</v>
@@ -11271,7 +11283,7 @@
         <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D51" t="n">
         <v>0.205257624111025</v>
@@ -11291,7 +11303,7 @@
         <v>6</v>
       </c>
       <c r="C52" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D52" t="n">
         <v>0.0590956884622356</v>
@@ -11311,7 +11323,7 @@
         <v>12</v>
       </c>
       <c r="C53" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D53" t="n">
         <v>0.855192387582626</v>
@@ -11331,7 +11343,7 @@
         <v>12</v>
       </c>
       <c r="C54" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D54" t="n">
         <v>0.103847744788657</v>
@@ -11351,7 +11363,7 @@
         <v>12</v>
       </c>
       <c r="C55" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D55" t="n">
         <v>0.0409598676287174</v>
@@ -11371,7 +11383,7 @@
         <v>6</v>
       </c>
       <c r="C56" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D56" t="n">
         <v>0.755545889300809</v>
@@ -11391,7 +11403,7 @@
         <v>6</v>
       </c>
       <c r="C57" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D57" t="n">
         <v>0.189430187423025</v>
@@ -11411,7 +11423,7 @@
         <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D58" t="n">
         <v>0.0550239232761654</v>
@@ -11431,7 +11443,7 @@
         <v>12</v>
       </c>
       <c r="C59" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D59" t="n">
         <v>0.828850368505133</v>
@@ -11451,7 +11463,7 @@
         <v>12</v>
       </c>
       <c r="C60" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D60" t="n">
         <v>0.11854951196471</v>
@@ -11471,7 +11483,7 @@
         <v>12</v>
       </c>
       <c r="C61" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D61" t="n">
         <v>0.0526001195301568</v>
@@ -11491,7 +11503,7 @@
         <v>6</v>
       </c>
       <c r="C62" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D62" t="n">
         <v>0.758941012393561</v>
@@ -11511,7 +11523,7 @@
         <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D63" t="n">
         <v>0.186948444492327</v>
@@ -11531,7 +11543,7 @@
         <v>6</v>
       </c>
       <c r="C64" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D64" t="n">
         <v>0.0541105431141123</v>
@@ -11551,7 +11563,7 @@
         <v>12</v>
       </c>
       <c r="C65" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D65" t="n">
         <v>0.829273285456141</v>
@@ -11571,7 +11583,7 @@
         <v>12</v>
       </c>
       <c r="C66" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D66" t="n">
         <v>0.12671443192203</v>
@@ -11591,7 +11603,7 @@
         <v>12</v>
       </c>
       <c r="C67" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D67" t="n">
         <v>0.0440122826218297</v>
@@ -11611,7 +11623,7 @@
         <v>6</v>
       </c>
       <c r="C68" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D68" t="n">
         <v>0.763987137975697</v>
@@ -11631,7 +11643,7 @@
         <v>6</v>
       </c>
       <c r="C69" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D69" t="n">
         <v>0.171275455578331</v>
@@ -11651,7 +11663,7 @@
         <v>6</v>
       </c>
       <c r="C70" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D70" t="n">
         <v>0.0647374064459713</v>
@@ -11671,7 +11683,7 @@
         <v>12</v>
       </c>
       <c r="C71" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D71" t="n">
         <v>0.852760736239257</v>
@@ -11691,7 +11703,7 @@
         <v>12</v>
       </c>
       <c r="C72" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D72" t="n">
         <v>0.112012665386811</v>
@@ -11711,7 +11723,7 @@
         <v>12</v>
       </c>
       <c r="C73" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D73" t="n">
         <v>0.0352265983739324</v>
@@ -11731,7 +11743,7 @@
         <v>6</v>
       </c>
       <c r="C74" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D74" t="n">
         <v>0.767135135287333</v>
@@ -11751,7 +11763,7 @@
         <v>6</v>
       </c>
       <c r="C75" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D75" t="n">
         <v>0.182918918785604</v>
@@ -11771,7 +11783,7 @@
         <v>6</v>
       </c>
       <c r="C76" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D76" t="n">
         <v>0.0499459459270629</v>
@@ -11791,7 +11803,7 @@
         <v>12</v>
       </c>
       <c r="C77" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D77" t="n">
         <v>0.831231814174975</v>
@@ -11811,7 +11823,7 @@
         <v>12</v>
       </c>
       <c r="C78" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D78" t="n">
         <v>0.130164888135845</v>
@@ -11831,7 +11843,7 @@
         <v>12</v>
       </c>
       <c r="C79" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D79" t="n">
         <v>0.0386032976891795</v>
@@ -11851,7 +11863,7 @@
         <v>6</v>
       </c>
       <c r="C80" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D80" t="n">
         <v>0.759011847784136</v>
@@ -11871,7 +11883,7 @@
         <v>6</v>
       </c>
       <c r="C81" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D81" t="n">
         <v>0.178472397574848</v>
@@ -11891,7 +11903,7 @@
         <v>6</v>
       </c>
       <c r="C82" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D82" t="n">
         <v>0.0625157546410162</v>
@@ -11911,7 +11923,7 @@
         <v>12</v>
       </c>
       <c r="C83" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D83" t="n">
         <v>0.862292879221022</v>
@@ -11931,7 +11943,7 @@
         <v>12</v>
       </c>
       <c r="C84" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D84" t="n">
         <v>0.0915808331764158</v>
@@ -11951,7 +11963,7 @@
         <v>12</v>
       </c>
       <c r="C85" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D85" t="n">
         <v>0.0461262876025623</v>
@@ -11971,7 +11983,7 @@
         <v>6</v>
       </c>
       <c r="C86" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D86" t="n">
         <v>0.759137055404775</v>
@@ -11991,7 +12003,7 @@
         <v>6</v>
       </c>
       <c r="C87" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D87" t="n">
         <v>0.190101523009983</v>
@@ -12011,7 +12023,7 @@
         <v>6</v>
       </c>
       <c r="C88" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D88" t="n">
         <v>0.0507614215852423</v>
@@ -12031,7 +12043,7 @@
         <v>12</v>
       </c>
       <c r="C89" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D89" t="n">
         <v>0.843604492030752</v>
@@ -12051,7 +12063,7 @@
         <v>12</v>
       </c>
       <c r="C90" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D90" t="n">
         <v>0.119967132204344</v>
@@ -12071,7 +12083,7 @@
         <v>12</v>
       </c>
       <c r="C91" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D91" t="n">
         <v>0.0364283757649041</v>
@@ -12091,7 +12103,7 @@
         <v>6</v>
       </c>
       <c r="C92" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D92" t="n">
         <v>0.737618545776891</v>
@@ -12111,7 +12123,7 @@
         <v>6</v>
       </c>
       <c r="C93" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D93" t="n">
         <v>0.220758693328011</v>
@@ -12131,7 +12143,7 @@
         <v>6</v>
       </c>
       <c r="C94" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D94" t="n">
         <v>0.0416227608950989</v>
@@ -12151,7 +12163,7 @@
         <v>12</v>
       </c>
       <c r="C95" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D95" t="n">
         <v>0.828480677536292</v>
@@ -12171,7 +12183,7 @@
         <v>12</v>
       </c>
       <c r="C96" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D96" t="n">
         <v>0.142138697517287</v>
@@ -12191,7 +12203,7 @@
         <v>12</v>
       </c>
       <c r="C97" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D97" t="n">
         <v>0.0293806249464208</v>
@@ -12211,7 +12223,7 @@
         <v>6</v>
       </c>
       <c r="C98" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D98" t="n">
         <v>0.767219567180595</v>
@@ -12231,7 +12243,7 @@
         <v>6</v>
       </c>
       <c r="C99" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D99" t="n">
         <v>0.185830755891598</v>
@@ -12251,7 +12263,7 @@
         <v>6</v>
       </c>
       <c r="C100" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D100" t="n">
         <v>0.0469496769278067</v>
@@ -12271,7 +12283,7 @@
         <v>12</v>
       </c>
       <c r="C101" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D101" t="n">
         <v>0.869276218403878</v>
@@ -12291,7 +12303,7 @@
         <v>12</v>
       </c>
       <c r="C102" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D102" t="n">
         <v>0.0969965537009361</v>
@@ -12311,7 +12323,7 @@
         <v>12</v>
       </c>
       <c r="C103" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D103" t="n">
         <v>0.0337272278951854</v>
@@ -12331,7 +12343,7 @@
         <v>6</v>
       </c>
       <c r="C104" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D104" t="n">
         <v>0.78554021161973</v>
@@ -12351,7 +12363,7 @@
         <v>6</v>
       </c>
       <c r="C105" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D105" t="n">
         <v>0.170863795988739</v>
@@ -12371,7 +12383,7 @@
         <v>6</v>
       </c>
       <c r="C106" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D106" t="n">
         <v>0.0435959923915308</v>
@@ -12391,7 +12403,7 @@
         <v>12</v>
       </c>
       <c r="C107" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D107" t="n">
         <v>0.836951034348865</v>
@@ -12411,7 +12423,7 @@
         <v>12</v>
       </c>
       <c r="C108" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D108" t="n">
         <v>0.120646138696426</v>
@@ -12431,7 +12443,7 @@
         <v>12</v>
       </c>
       <c r="C109" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D109" t="n">
         <v>0.0424028269547087</v>
@@ -12451,7 +12463,7 @@
         <v>6</v>
       </c>
       <c r="C110" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D110" t="n">
         <v>0.802752293842932</v>
@@ -12471,7 +12483,7 @@
         <v>6</v>
       </c>
       <c r="C111" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D111" t="n">
         <v>0.157396788844894</v>
@@ -12491,7 +12503,7 @@
         <v>6</v>
       </c>
       <c r="C112" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D112" t="n">
         <v>0.0398509173121742</v>
@@ -12511,7 +12523,7 @@
         <v>12</v>
       </c>
       <c r="C113" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D113" t="n">
         <v>0.851497608838443</v>
@@ -12531,7 +12543,7 @@
         <v>12</v>
       </c>
       <c r="C114" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D114" t="n">
         <v>0.111754341773604</v>
@@ -12551,7 +12563,7 @@
         <v>12</v>
       </c>
       <c r="C115" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D115" t="n">
         <v>0.0367480493879525</v>
@@ -12571,7 +12583,7 @@
         <v>6</v>
       </c>
       <c r="C116" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D116" t="n">
         <v>0.784958217174832</v>
@@ -12591,7 +12603,7 @@
         <v>6</v>
       </c>
       <c r="C117" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D117" t="n">
         <v>0.178551531987225</v>
@@ -12611,7 +12623,7 @@
         <v>6</v>
       </c>
       <c r="C118" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D118" t="n">
         <v>0.0364902508379434</v>
@@ -12631,7 +12643,7 @@
         <v>12</v>
       </c>
       <c r="C119" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D119" t="n">
         <v>0.851347946656267</v>
@@ -12651,7 +12663,7 @@
         <v>12</v>
       </c>
       <c r="C120" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D120" t="n">
         <v>0.114134542301303</v>
@@ -12671,7 +12683,7 @@
         <v>12</v>
       </c>
       <c r="C121" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D121" t="n">
         <v>0.0345175110424291</v>
@@ -12691,7 +12703,7 @@
         <v>6</v>
       </c>
       <c r="C122" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D122" t="n">
         <v>0.790130261195659</v>
@@ -12711,7 +12723,7 @@
         <v>6</v>
       </c>
       <c r="C123" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D123" t="n">
         <v>0.174853051974447</v>
@@ -12731,7 +12743,7 @@
         <v>6</v>
       </c>
       <c r="C124" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D124" t="n">
         <v>0.0350166868298947</v>
@@ -12751,7 +12763,7 @@
         <v>12</v>
       </c>
       <c r="C125" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D125" t="n">
         <v>0.846957570286449</v>
@@ -12771,7 +12783,7 @@
         <v>12</v>
       </c>
       <c r="C126" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D126" t="n">
         <v>0.116722615872122</v>
@@ -12791,7 +12803,7 @@
         <v>12</v>
       </c>
       <c r="C127" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D127" t="n">
         <v>0.0363198138414282</v>
@@ -12811,7 +12823,7 @@
         <v>6</v>
       </c>
       <c r="C128" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D128" t="n">
         <v>0.789781839330301</v>
@@ -12831,7 +12843,7 @@
         <v>6</v>
       </c>
       <c r="C129" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D129" t="n">
         <v>0.178232439882754</v>
@@ -12851,7 +12863,7 @@
         <v>6</v>
       </c>
       <c r="C130" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D130" t="n">
         <v>0.0319857207869448</v>
@@ -12871,7 +12883,7 @@
         <v>12</v>
       </c>
       <c r="C131" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D131" t="n">
         <v>0.819084596312256</v>
@@ -12891,7 +12903,7 @@
         <v>12</v>
       </c>
       <c r="C132" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D132" t="n">
         <v>0.126795332452439</v>
@@ -12911,7 +12923,7 @@
         <v>12</v>
       </c>
       <c r="C133" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D133" t="n">
         <v>0.0541200712353049</v>
@@ -12931,7 +12943,7 @@
         <v>6</v>
       </c>
       <c r="C134" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D134" t="n">
         <v>0.80564632982896</v>
@@ -12951,7 +12963,7 @@
         <v>6</v>
       </c>
       <c r="C135" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D135" t="n">
         <v>0.160950363282832</v>
@@ -12971,7 +12983,7 @@
         <v>6</v>
       </c>
       <c r="C136" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D136" t="n">
         <v>0.0334033068882076</v>
@@ -12991,7 +13003,7 @@
         <v>12</v>
       </c>
       <c r="C137" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D137" t="n">
         <v>0.838894559140156</v>
@@ -13011,7 +13023,7 @@
         <v>12</v>
       </c>
       <c r="C138" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D138" t="n">
         <v>0.12528293577161</v>
@@ -13031,7 +13043,7 @@
         <v>12</v>
       </c>
       <c r="C139" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D139" t="n">
         <v>0.0358225050882343</v>
@@ -13051,7 +13063,7 @@
         <v>6</v>
       </c>
       <c r="C140" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D140" t="n">
         <v>0.815365529855667</v>
@@ -13071,7 +13083,7 @@
         <v>6</v>
       </c>
       <c r="C141" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D141" t="n">
         <v>0.152834504927022</v>
@@ -13091,7 +13103,7 @@
         <v>6</v>
       </c>
       <c r="C142" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D142" t="n">
         <v>0.0317999652173109</v>
@@ -13111,7 +13123,7 @@
         <v>12</v>
       </c>
       <c r="C143" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D143" t="n">
         <v>0.861607304194992</v>
@@ -13131,7 +13143,7 @@
         <v>12</v>
       </c>
       <c r="C144" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D144" t="n">
         <v>0.105257948390904</v>
@@ -13151,7 +13163,7 @@
         <v>12</v>
       </c>
       <c r="C145" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D145" t="n">
         <v>0.0331347474141034</v>
@@ -13171,7 +13183,7 @@
         <v>6</v>
       </c>
       <c r="C146" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D146" t="n">
         <v>0.783062894713988</v>
@@ -13191,7 +13203,7 @@
         <v>6</v>
       </c>
       <c r="C147" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D147" t="n">
         <v>0.172702319714057</v>
@@ -13211,7 +13223,7 @@
         <v>6</v>
       </c>
       <c r="C148" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D148" t="n">
         <v>0.0442347855719549</v>
@@ -13231,7 +13243,7 @@
         <v>12</v>
       </c>
       <c r="C149" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D149" t="n">
         <v>0.866018017092901</v>
@@ -13251,7 +13263,7 @@
         <v>12</v>
       </c>
       <c r="C150" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D150" t="n">
         <v>0.102468232459954</v>
@@ -13271,7 +13283,7 @@
         <v>12</v>
       </c>
       <c r="C151" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D151" t="n">
         <v>0.0315137504471447</v>
@@ -13291,7 +13303,7 @@
         <v>6</v>
       </c>
       <c r="C152" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D152" t="n">
         <v>0.801927184755855</v>
@@ -13311,7 +13323,7 @@
         <v>6</v>
       </c>
       <c r="C153" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D153" t="n">
         <v>0.151756770729616</v>
@@ -13331,7 +13343,7 @@
         <v>6</v>
       </c>
       <c r="C154" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D154" t="n">
         <v>0.0463160445145284</v>
@@ -13351,7 +13363,7 @@
         <v>12</v>
       </c>
       <c r="C155" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D155" t="n">
         <v>0.832220683393028</v>
@@ -13371,7 +13383,7 @@
         <v>12</v>
       </c>
       <c r="C156" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D156" t="n">
         <v>0.128484198530179</v>
@@ -13391,7 +13403,7 @@
         <v>12</v>
       </c>
       <c r="C157" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D157" t="n">
         <v>0.0392951180767933</v>
@@ -13411,7 +13423,7 @@
         <v>6</v>
       </c>
       <c r="C158" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D158" t="n">
         <v>0.795940531732115</v>
@@ -13431,7 +13443,7 @@
         <v>6</v>
       </c>
       <c r="C159" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D159" t="n">
         <v>0.174245239174463</v>
@@ -13451,7 +13463,7 @@
         <v>6</v>
       </c>
       <c r="C160" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D160" t="n">
         <v>0.0298142290934228</v>
@@ -13471,7 +13483,7 @@
         <v>12</v>
       </c>
       <c r="C161" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D161" t="n">
         <v>0.8822684902293</v>
@@ -13491,7 +13503,7 @@
         <v>12</v>
       </c>
       <c r="C162" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D162" t="n">
         <v>0.10138654702909</v>
@@ -13511,7 +13523,7 @@
         <v>12</v>
       </c>
       <c r="C163" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D163" t="n">
         <v>0.0163449627416108</v>
@@ -13531,7 +13543,7 @@
         <v>6</v>
       </c>
       <c r="C164" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D164" t="n">
         <v>0.78543055017164</v>
@@ -13551,7 +13563,7 @@
         <v>6</v>
       </c>
       <c r="C165" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D165" t="n">
         <v>0.194268619188887</v>
@@ -13571,7 +13583,7 @@
         <v>6</v>
       </c>
       <c r="C166" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D166" t="n">
         <v>0.020300830639473</v>
@@ -13591,7 +13603,7 @@
         <v>12</v>
       </c>
       <c r="C167" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D167" t="n">
         <v>0.850550242106477</v>
@@ -13611,7 +13623,7 @@
         <v>12</v>
       </c>
       <c r="C168" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D168" t="n">
         <v>0.119439549639988</v>
@@ -13631,7 +13643,7 @@
         <v>12</v>
       </c>
       <c r="C169" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D169" t="n">
         <v>0.0300102082535351</v>
@@ -13651,7 +13663,7 @@
         <v>6</v>
       </c>
       <c r="C170" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D170" t="n">
         <v>0.789184764008818</v>
@@ -13671,7 +13683,7 @@
         <v>6</v>
       </c>
       <c r="C171" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D171" t="n">
         <v>0.177488088932764</v>
@@ -13691,7 +13703,7 @@
         <v>6</v>
       </c>
       <c r="C172" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D172" t="n">
         <v>0.033327147058418</v>
@@ -13711,7 +13723,7 @@
         <v>12</v>
       </c>
       <c r="C173" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D173" t="n">
         <v>0.865714485414053</v>
@@ -13731,7 +13743,7 @@
         <v>12</v>
       </c>
       <c r="C174" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D174" t="n">
         <v>0.105617453881076</v>
@@ -13751,7 +13763,7 @@
         <v>12</v>
       </c>
       <c r="C175" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D175" t="n">
         <v>0.0286680607048707</v>
@@ -13771,7 +13783,7 @@
         <v>6</v>
       </c>
       <c r="C176" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D176" t="n">
         <v>0.824650207939676</v>
@@ -13791,7 +13803,7 @@
         <v>6</v>
       </c>
       <c r="C177" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D177" t="n">
         <v>0.143322989592271</v>
@@ -13811,7 +13823,7 @@
         <v>6</v>
       </c>
       <c r="C178" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D178" t="n">
         <v>0.0320268024680526</v>
@@ -13831,7 +13843,7 @@
         <v>12</v>
       </c>
       <c r="C179" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D179" t="n">
         <v>0.884925858858901</v>
@@ -13851,7 +13863,7 @@
         <v>12</v>
       </c>
       <c r="C180" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D180" t="n">
         <v>0.0906221348270612</v>
@@ -13871,7 +13883,7 @@
         <v>12</v>
       </c>
       <c r="C181" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D181" t="n">
         <v>0.0244520063140374</v>
@@ -13891,7 +13903,7 @@
         <v>6</v>
       </c>
       <c r="C182" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D182" t="n">
         <v>0.836147265920846</v>
@@ -13911,7 +13923,7 @@
         <v>6</v>
       </c>
       <c r="C183" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D183" t="n">
         <v>0.123880928758985</v>
@@ -13931,7 +13943,7 @@
         <v>6</v>
       </c>
       <c r="C184" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D184" t="n">
         <v>0.0399718053201691</v>
@@ -13951,7 +13963,7 @@
         <v>12</v>
       </c>
       <c r="C185" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D185" t="n">
         <v>0.838688747232041</v>
@@ -13971,7 +13983,7 @@
         <v>12</v>
       </c>
       <c r="C186" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D186" t="n">
         <v>0.129882161555719</v>
@@ -13991,7 +14003,7 @@
         <v>12</v>
       </c>
       <c r="C187" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D187" t="n">
         <v>0.03142909121224</v>
@@ -14011,7 +14023,7 @@
         <v>6</v>
       </c>
       <c r="C188" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D188" t="n">
         <v>0.841165644233526</v>
@@ -14031,7 +14043,7 @@
         <v>6</v>
       </c>
       <c r="C189" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D189" t="n">
         <v>0.122363687122403</v>
@@ -14051,7 +14063,7 @@
         <v>6</v>
       </c>
       <c r="C190" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D190" t="n">
         <v>0.0364706686440712</v>
@@ -14071,7 +14083,7 @@
         <v>12</v>
       </c>
       <c r="C191" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D191" t="n">
         <v>0.850020790079998</v>
@@ -14091,7 +14103,7 @@
         <v>12</v>
       </c>
       <c r="C192" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D192" t="n">
         <v>0.121602640160722</v>
@@ -14111,7 +14123,7 @@
         <v>12</v>
       </c>
       <c r="C193" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D193" t="n">
         <v>0.0283765697592797</v>
@@ -14131,7 +14143,7 @@
         <v>6</v>
       </c>
       <c r="C194" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D194" t="n">
         <v>0.804347249155249</v>
@@ -14151,7 +14163,7 @@
         <v>6</v>
       </c>
       <c r="C195" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D195" t="n">
         <v>0.153505992721089</v>
@@ -14171,7 +14183,7 @@
         <v>6</v>
       </c>
       <c r="C196" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D196" t="n">
         <v>0.0421467581236617</v>
@@ -14191,7 +14203,7 @@
         <v>12</v>
       </c>
       <c r="C197" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D197" t="n">
         <v>0.866396927842532</v>
@@ -14211,7 +14223,7 @@
         <v>12</v>
       </c>
       <c r="C198" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D198" t="n">
         <v>0.097560886100472</v>
@@ -14231,7 +14243,7 @@
         <v>12</v>
       </c>
       <c r="C199" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D199" t="n">
         <v>0.0360421860569962</v>
@@ -14251,7 +14263,7 @@
         <v>6</v>
       </c>
       <c r="C200" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D200" t="n">
         <v>0.810946283337422</v>
@@ -14271,7 +14283,7 @@
         <v>6</v>
       </c>
       <c r="C201" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D201" t="n">
         <v>0.152923140358873</v>
@@ -14291,7 +14303,7 @@
         <v>6</v>
       </c>
       <c r="C202" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D202" t="n">
         <v>0.0361305763037056</v>
@@ -14311,7 +14323,7 @@
         <v>12</v>
       </c>
       <c r="C203" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D203" t="n">
         <v>0.859771571463655</v>
@@ -14331,7 +14343,7 @@
         <v>12</v>
       </c>
       <c r="C204" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D204" t="n">
         <v>0.109965811537771</v>
@@ -14351,7 +14363,7 @@
         <v>12</v>
       </c>
       <c r="C205" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D205" t="n">
         <v>0.030262616998574</v>
@@ -14371,7 +14383,7 @@
         <v>6</v>
       </c>
       <c r="C206" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D206" t="n">
         <v>0.780359247691811</v>
@@ -14391,7 +14403,7 @@
         <v>6</v>
       </c>
       <c r="C207" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D207" t="n">
         <v>0.178843485130728</v>
@@ -14411,7 +14423,7 @@
         <v>6</v>
       </c>
       <c r="C208" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D208" t="n">
         <v>0.0407972671774604</v>
@@ -14431,7 +14443,7 @@
         <v>12</v>
       </c>
       <c r="C209" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D209" t="n">
         <v>0.853432664863191</v>
@@ -14451,7 +14463,7 @@
         <v>12</v>
       </c>
       <c r="C210" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D210" t="n">
         <v>0.106232187128298</v>
@@ -14471,7 +14483,7 @@
         <v>12</v>
       </c>
       <c r="C211" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D211" t="n">
         <v>0.0403351480085117</v>
@@ -14491,7 +14503,7 @@
         <v>6</v>
       </c>
       <c r="C212" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D212" t="n">
         <v>0.775133341331462</v>
@@ -14511,7 +14523,7 @@
         <v>6</v>
       </c>
       <c r="C213" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D213" t="n">
         <v>0.182126124693067</v>
@@ -14531,7 +14543,7 @@
         <v>6</v>
       </c>
       <c r="C214" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D214" t="n">
         <v>0.0427405339754717</v>
@@ -14551,7 +14563,7 @@
         <v>12</v>
       </c>
       <c r="C215" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D215" t="n">
         <v>0.840195152504289</v>
@@ -14571,7 +14583,7 @@
         <v>12</v>
       </c>
       <c r="C216" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D216" t="n">
         <v>0.124125734815184</v>
@@ -14591,7 +14603,7 @@
         <v>12</v>
       </c>
       <c r="C217" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D217" t="n">
         <v>0.0356791126805267</v>
@@ -14611,7 +14623,7 @@
         <v>6</v>
       </c>
       <c r="C218" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D218" t="n">
         <v>0.802952305820162</v>
@@ -14631,7 +14643,7 @@
         <v>6</v>
       </c>
       <c r="C219" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D219" t="n">
         <v>0.150942687772203</v>
@@ -14651,7 +14663,7 @@
         <v>6</v>
       </c>
       <c r="C220" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D220" t="n">
         <v>0.046105006407635</v>
@@ -14671,7 +14683,7 @@
         <v>12</v>
       </c>
       <c r="C221" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D221" t="n">
         <v>0.875464714661557</v>
@@ -14691,7 +14703,7 @@
         <v>12</v>
       </c>
       <c r="C222" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D222" t="n">
         <v>0.0939442544180007</v>
@@ -14711,7 +14723,7 @@
         <v>12</v>
       </c>
       <c r="C223" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D223" t="n">
         <v>0.0305910309204428</v>
@@ -14731,7 +14743,7 @@
         <v>6</v>
       </c>
       <c r="C224" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D224" t="n">
         <v>0.787980778540685</v>
@@ -14751,7 +14763,7 @@
         <v>6</v>
       </c>
       <c r="C225" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D225" t="n">
         <v>0.169836234573126</v>
@@ -14771,7 +14783,7 @@
         <v>6</v>
       </c>
       <c r="C226" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D226" t="n">
         <v>0.0421829868861893</v>
@@ -14791,7 +14803,7 @@
         <v>12</v>
       </c>
       <c r="C227" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D227" t="n">
         <v>0.834822443999278</v>
@@ -14811,7 +14823,7 @@
         <v>12</v>
       </c>
       <c r="C228" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D228" t="n">
         <v>0.125996596843156</v>
@@ -14831,7 +14843,7 @@
         <v>12</v>
       </c>
       <c r="C229" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D229" t="n">
         <v>0.0391809591575662</v>
@@ -14851,7 +14863,7 @@
         <v>6</v>
       </c>
       <c r="C230" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D230" t="n">
         <v>0.796964438043496</v>
@@ -14871,7 +14883,7 @@
         <v>6</v>
       </c>
       <c r="C231" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D231" t="n">
         <v>0.164604952028703</v>
@@ -14891,7 +14903,7 @@
         <v>6</v>
       </c>
       <c r="C232" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D232" t="n">
         <v>0.0384306099278011</v>
@@ -14911,7 +14923,7 @@
         <v>12</v>
       </c>
       <c r="C233" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D233" t="n">
         <v>0.830783139698313</v>
@@ -14931,7 +14943,7 @@
         <v>12</v>
       </c>
       <c r="C234" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D234" t="n">
         <v>0.134691371999022</v>
@@ -14951,7 +14963,7 @@
         <v>12</v>
       </c>
       <c r="C235" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D235" t="n">
         <v>0.0345254883026649</v>
@@ -14971,7 +14983,7 @@
         <v>6</v>
       </c>
       <c r="C236" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D236" t="n">
         <v>0.77799850464152</v>
@@ -14991,7 +15003,7 @@
         <v>6</v>
       </c>
       <c r="C237" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D237" t="n">
         <v>0.177743268769115</v>
@@ -15011,7 +15023,7 @@
         <v>6</v>
       </c>
       <c r="C238" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D238" t="n">
         <v>0.0442582265893646</v>
@@ -15031,7 +15043,7 @@
         <v>12</v>
       </c>
       <c r="C239" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D239" t="n">
         <v>0.817536754542111</v>
@@ -15051,7 +15063,7 @@
         <v>12</v>
       </c>
       <c r="C240" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D240" t="n">
         <v>0.138283142901079</v>
@@ -15071,7 +15083,7 @@
         <v>12</v>
       </c>
       <c r="C241" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D241" t="n">
         <v>0.0441801025568104</v>
@@ -15091,7 +15103,7 @@
         <v>6</v>
       </c>
       <c r="C242" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D242" t="n">
         <v>0.754907777021095</v>
@@ -15111,7 +15123,7 @@
         <v>6</v>
       </c>
       <c r="C243" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D243" t="n">
         <v>0.204038588962721</v>
@@ -15131,7 +15143,7 @@
         <v>6</v>
       </c>
       <c r="C244" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D244" t="n">
         <v>0.0410536340161836</v>
@@ -15151,7 +15163,7 @@
         <v>12</v>
       </c>
       <c r="C245" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D245" t="n">
         <v>0.813631914909185</v>
@@ -15171,7 +15183,7 @@
         <v>12</v>
       </c>
       <c r="C246" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D246" t="n">
         <v>0.134815923936203</v>
@@ -15191,7 +15203,7 @@
         <v>12</v>
       </c>
       <c r="C247" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D247" t="n">
         <v>0.0515521611546121</v>
@@ -15211,7 +15223,7 @@
         <v>6</v>
       </c>
       <c r="C248" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D248" t="n">
         <v>0.774724828155531</v>
@@ -15231,7 +15243,7 @@
         <v>6</v>
       </c>
       <c r="C249" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D249" t="n">
         <v>0.18817421730421</v>
@@ -15251,7 +15263,7 @@
         <v>6</v>
       </c>
       <c r="C250" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D250" t="n">
         <v>0.0371009545402584</v>
@@ -15271,7 +15283,7 @@
         <v>12</v>
       </c>
       <c r="C251" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D251" t="n">
         <v>0.815773349145219</v>
@@ -15291,7 +15303,7 @@
         <v>12</v>
       </c>
       <c r="C252" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D252" t="n">
         <v>0.133766078844108</v>
@@ -15311,7 +15323,7 @@
         <v>12</v>
       </c>
       <c r="C253" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D253" t="n">
         <v>0.0504605720106725</v>
@@ -15331,7 +15343,7 @@
         <v>6</v>
       </c>
       <c r="C254" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D254" t="n">
         <v>0.777811771876306</v>
@@ -15351,7 +15363,7 @@
         <v>6</v>
       </c>
       <c r="C255" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D255" t="n">
         <v>0.193503265996483</v>
@@ -15371,7 +15383,7 @@
         <v>6</v>
       </c>
       <c r="C256" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D256" t="n">
         <v>0.0286849621272115</v>
@@ -15391,7 +15403,7 @@
         <v>12</v>
       </c>
       <c r="C257" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D257" t="n">
         <v>0.795302193121186</v>
@@ -15411,7 +15423,7 @@
         <v>12</v>
       </c>
       <c r="C258" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D258" t="n">
         <v>0.163671052001334</v>
@@ -15431,7 +15443,7 @@
         <v>12</v>
       </c>
       <c r="C259" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D259" t="n">
         <v>0.0410267548774796</v>
@@ -15451,7 +15463,7 @@
         <v>6</v>
       </c>
       <c r="C260" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D260" t="n">
         <v>0.790628994985912</v>
@@ -15471,7 +15483,7 @@
         <v>6</v>
       </c>
       <c r="C261" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D261" t="n">
         <v>0.167143662980272</v>
@@ -15491,7 +15503,7 @@
         <v>6</v>
       </c>
       <c r="C262" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D262" t="n">
         <v>0.0422273420338155</v>
@@ -15511,7 +15523,7 @@
         <v>12</v>
       </c>
       <c r="C263" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D263" t="n">
         <v>0.783000037765092</v>
@@ -15531,7 +15543,7 @@
         <v>12</v>
       </c>
       <c r="C264" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D264" t="n">
         <v>0.169743745233129</v>
@@ -15551,7 +15563,7 @@
         <v>12</v>
       </c>
       <c r="C265" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D265" t="n">
         <v>0.0472562170017787</v>
@@ -15571,7 +15583,7 @@
         <v>6</v>
       </c>
       <c r="C266" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D266" t="n">
         <v>0.724480114531782</v>
@@ -15591,7 +15603,7 @@
         <v>6</v>
       </c>
       <c r="C267" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D267" t="n">
         <v>0.228762638480078</v>
@@ -15611,7 +15623,7 @@
         <v>6</v>
       </c>
       <c r="C268" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D268" t="n">
         <v>0.0467572469881401</v>
@@ -15631,7 +15643,7 @@
         <v>12</v>
       </c>
       <c r="C269" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D269" t="n">
         <v>0.74223597790077</v>
@@ -15651,7 +15663,7 @@
         <v>12</v>
       </c>
       <c r="C270" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D270" t="n">
         <v>0.182498413890673</v>
@@ -15671,7 +15683,7 @@
         <v>12</v>
       </c>
       <c r="C271" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D271" t="n">
         <v>0.0752656082085574</v>
@@ -15691,7 +15703,7 @@
         <v>6</v>
       </c>
       <c r="C272" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D272" t="n">
         <v>0.745458546645622</v>
@@ -15711,7 +15723,7 @@
         <v>6</v>
       </c>
       <c r="C273" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D273" t="n">
         <v>0.175781137419641</v>
@@ -15731,7 +15743,7 @@
         <v>6</v>
       </c>
       <c r="C274" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D274" t="n">
         <v>0.078760315934737</v>
@@ -15751,7 +15763,7 @@
         <v>12</v>
       </c>
       <c r="C275" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D275" t="n">
         <v>0.694946755873342</v>
@@ -15771,7 +15783,7 @@
         <v>12</v>
       </c>
       <c r="C276" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D276" t="n">
         <v>0.180072534954597</v>
@@ -15791,7 +15803,7 @@
         <v>12</v>
       </c>
       <c r="C277" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D277" t="n">
         <v>0.124980709172061</v>
@@ -15811,7 +15823,7 @@
         <v>6</v>
       </c>
       <c r="C278" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D278" t="n">
         <v>0.733469858934396</v>
@@ -15831,7 +15843,7 @@
         <v>6</v>
       </c>
       <c r="C279" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D279" t="n">
         <v>0.212649914067923</v>
@@ -15851,7 +15863,7 @@
         <v>6</v>
       </c>
       <c r="C280" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D280" t="n">
         <v>0.0538802269976803</v>
@@ -15871,7 +15883,7 @@
         <v>12</v>
       </c>
       <c r="C281" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D281" t="n">
         <v>0.731991604051296</v>
@@ -15891,7 +15903,7 @@
         <v>12</v>
       </c>
       <c r="C282" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D282" t="n">
         <v>0.204306622172829</v>
@@ -15911,7 +15923,7 @@
         <v>12</v>
       </c>
       <c r="C283" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D283" t="n">
         <v>0.063701773775875</v>
@@ -15942,31 +15954,31 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2">
@@ -15974,7 +15986,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C2" t="n">
         <v>0.802952305820162</v>
@@ -15998,7 +16010,7 @@
         <v>-0.0694824468857661</v>
       </c>
       <c r="J2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3">
@@ -16006,7 +16018,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C3" t="n">
         <v>0.150942687772203</v>
@@ -16030,7 +16042,7 @@
         <v>0.0617072262957207</v>
       </c>
       <c r="J3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4">
@@ -16038,7 +16050,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C4" t="n">
         <v>0.046105006407635</v>
@@ -16062,7 +16074,7 @@
         <v>0.00777522059004531</v>
       </c>
       <c r="J4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
@@ -16070,7 +16082,7 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C5" t="n">
         <v>0.875464714661557</v>
@@ -16094,7 +16106,7 @@
         <v>-0.14347311061026</v>
       </c>
       <c r="J5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6">
@@ -16102,7 +16114,7 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C6" t="n">
         <v>0.0939442544180007</v>
@@ -16126,7 +16138,7 @@
         <v>0.110362367754828</v>
       </c>
       <c r="J6" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7">
@@ -16134,7 +16146,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C7" t="n">
         <v>0.0305910309204428</v>
@@ -16158,7 +16170,7 @@
         <v>0.0331107428554322</v>
       </c>
       <c r="J7" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>